<commit_message>
2o Set Askhsewn Oloklirwmeni 2 Erwtisi
</commit_message>
<xml_diff>
--- a/2h askhsh/double-diode2025-start example.xlsx
+++ b/2h askhsh/double-diode2025-start example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dimt\Documents\!!!Mathimata-Simeiwseis\PHYSICS AND TECHNOLOGY OF SEMICONDUCTOR DEVICES\2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalog\Documents\Φυσικη και Τεχνολογια Ημιαγωγικων Διαταξεων\ERGASIES\Fysikh-kai-Texnologia-Imiagwgwn\2h askhsh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7063C1F1-3C80-42D6-A90B-DBA15AD9EA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459C29F6-BDF3-468D-A0FB-55D099A4EBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="22180" windowHeight="11640" xr2:uid="{E6749CEB-4BB9-4780-BF49-BE23224B6481}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E6749CEB-4BB9-4780-BF49-BE23224B6481}"/>
   </bookViews>
   <sheets>
     <sheet name="ddiode" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7103,9 +7103,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>44450</xdr:colOff>
+          <xdr:colOff>45720</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>158750</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7263,9 +7263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7303,7 +7303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7409,7 +7409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7551,7 +7551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7561,13 +7561,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E58763-6C11-4B8F-B821-CA6378A68EFD}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.02</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>6.0699999999999997E-10</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.04</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>1.2030000000000001E-9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.06</v>
       </c>
@@ -7599,7 +7599,7 @@
         <v>2.1649999999999999E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.08</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>3.5079999999999999E-9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.1</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>5.4169999999999998E-9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.12</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>8.2100000000000004E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.14000000000000001</v>
       </c>
@@ -7631,7 +7631,7 @@
         <v>1.1830000000000001E-8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.16</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>1.7299999999999999E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.18</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>2.449E-8</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.2</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>3.4160000000000003E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.22</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>4.7640000000000002E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.24</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>6.5009999999999998E-8</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.26</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>8.8660000000000001E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.28000000000000003</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>1.209E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.3</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>1.666E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0.32</v>
       </c>
@@ -7703,7 +7703,7 @@
         <v>2.3050000000000001E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0.34</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>3.2010000000000001E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0.36</v>
       </c>
@@ -7719,7 +7719,7 @@
         <v>4.4620000000000001E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.38</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>6.285E-7</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0.4</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>8.8449999999999996E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0.42</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>1.249E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0.44</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>1.776E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0.46</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>2.5270000000000001E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0.48</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>3.6150000000000001E-6</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0.5</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>5.2000000000000002E-6</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0.52</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>7.576E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0.54</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>1.1219999999999999E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0.56000000000000005</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>1.7110000000000001E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0.57999999999999996</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>2.694E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0.6</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>4.426E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0.62</v>
       </c>
@@ -7823,7 +7823,7 @@
         <v>7.5779999999999996E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0.64</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>1.359E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0.66</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>2.5310000000000003E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0.68</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>4.8519999999999998E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0.7</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>9.4439999999999997E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0.72</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0.74</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>3.5200000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0.76</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>6.43E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0.78</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>1.103E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0.8</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>1.7520000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0.82</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0.84</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>3.5779999999999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0.86</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>4.7059999999999998E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0.88</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>5.9409999999999998E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0.9</v>
       </c>
@@ -7944,18 +7944,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2311FB37-D30C-4CD8-B994-E04144F5060E}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21">
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -7991,7 +7991,7 @@
         <v>1.0000000000000001E-15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7999,7 +7999,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -8009,7 +8009,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -8018,7 +8018,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.02</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>4.7179295264854998E-11</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.04</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>1.1661770908965958E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.06</v>
       </c>
@@ -8113,7 +8113,7 @@
         <v>2.1881762141740435E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.08</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>3.6923733968582682E-10</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.1</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>5.9063049676522627E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.12</v>
       </c>
@@ -8188,7 +8188,7 @@
         <v>9.1649063047591952E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0.14000000000000001</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>1.3961240948560971E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0.16</v>
       </c>
@@ -8226,11 +8226,11 @@
         <v>0.16</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
+        <f>E$2*(EXP($A18/E$1/$B$4)-1)</f>
         <v>2.1016395804180699E-9</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f>F$2*(EXP($A18/F$1/$B$4)-1)</f>
         <v>4.8372168420634567E-13</v>
       </c>
       <c r="G18" s="1">
@@ -8238,7 +8238,7 @@
         <v>2.1021233021022762E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0.18</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>3.1413809196389676E-9</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.2</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>0.2</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="1"/>
+        <f>E$2*(EXP($A20/E$1/$B$4)-1)</f>
         <v>4.6690599333857072E-9</v>
       </c>
       <c r="F20" s="1">
@@ -8288,7 +8288,7 @@
         <v>4.6713333266505298E-9</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0.22</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>0.22</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="1"/>
+        <f>E$2*(EXP($A21/E$1/$B$4)-1)</f>
         <v>6.9190131867920646E-9</v>
       </c>
       <c r="F21" s="1">
@@ -8313,7 +8313,7 @@
         <v>6.9239388414037009E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0.24</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>1.0241123115789899E-8</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0.26</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>1.5127282080135809E-8</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0.28000000000000003</v>
       </c>
@@ -8388,7 +8388,7 @@
         <v>2.2327280617262719E-8</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0.3</v>
       </c>
@@ -8413,7 +8413,7 @@
         <v>3.2942821784227835E-8</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0.32</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>4.8607122531774397E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0.34</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>7.1749375331870619E-8</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0.36</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>1.0599995784115163E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0.38</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>1.5682142779603311E-7</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0.4</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>2.3251219020531879E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0.42</v>
       </c>
@@ -8563,7 +8563,7 @@
         <v>3.4584609467717125E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0.44</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>5.1683738582596401E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0.46</v>
       </c>
@@ -8613,7 +8613,7 @@
         <v>7.7757220074672988E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0.48</v>
       </c>
@@ -8638,7 +8638,7 @@
         <v>1.1809702816201879E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0.5</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>1.8172561754553523E-6</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0.52</v>
       </c>
@@ -8688,7 +8688,7 @@
         <v>2.8459470843037869E-6</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0.54</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>4.5597105741929475E-6</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0.56000000000000005</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>7.5146939330075066E-6</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0.57999999999999996</v>
       </c>
@@ -8763,7 +8763,7 @@
         <v>1.2801068361593235E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0.6</v>
       </c>
@@ -8788,7 +8788,7 @@
         <v>2.2611746477015218E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0.62</v>
       </c>
@@ -8813,7 +8813,7 @@
         <v>4.1448814160022E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0.64</v>
       </c>
@@ -8838,7 +8838,7 @@
         <v>7.8699315363716423E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0.66</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>1.5415954818257441E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0.68</v>
       </c>
@@ -8888,7 +8888,7 @@
         <v>3.0992020025822785E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0.7</v>
       </c>
@@ -8913,7 +8913,7 @@
         <v>6.3599161484597603E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0.72</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>1.3256356793064543E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0.74</v>
       </c>
@@ -8961,7 +8961,7 @@
         <v>2.7949633742143749E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0.76</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>5.9416185236610269E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0.78</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>1.2704561860402841E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0.8</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>2.727581581548701E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0.82</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>5.8724057949470304E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0.84</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>0.12667590292645184</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0.86</v>
       </c>
@@ -9105,7 +9105,7 @@
         <v>0.27361972238058352</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0.88</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>0.59155356782512847</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0.9</v>
       </c>
@@ -9167,7 +9167,7 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9186,9 +9186,9 @@
               </from>
               <to>
                 <xdr:col>10</xdr:col>
-                <xdr:colOff>44450</xdr:colOff>
+                <xdr:colOff>45720</xdr:colOff>
                 <xdr:row>24</xdr:row>
-                <xdr:rowOff>158750</xdr:rowOff>
+                <xdr:rowOff>160020</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -9356,13 +9356,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EB5F384-A592-4519-966E-CBFB15E4E8BB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EB5F384-A592-4519-966E-CBFB15E4E8BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{088BC2DF-19C6-40D2-BBA8-BA193C858B25}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{088BC2DF-19C6-40D2-BBA8-BA193C858B25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0501531-E0EF-4E9F-9A95-88C9C9FAD15A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0501531-E0EF-4E9F-9A95-88C9C9FAD15A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a7907efa-e053-4288-b367-36de09e1d0a0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>